<commit_message>
layout halaman admin & user
</commit_message>
<xml_diff>
--- a/database/FileExcel/Article.xlsx
+++ b/database/FileExcel/Article.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yovie\persediaanapp-magang\database\FileExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEF196A-DC53-4F70-B4DF-AF37AB501AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B8649D8-BE2E-46A7-8703-E04EEC9B18B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="1100" windowWidth="11440" windowHeight="7810" xr2:uid="{B1A6D6DA-43F5-4D03-876B-1BE0E6BF7134}"/>
+    <workbookView xWindow="430" yWindow="410" windowWidth="11440" windowHeight="7810" xr2:uid="{B1A6D6DA-43F5-4D03-876B-1BE0E6BF7134}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>id</t>
   </si>
@@ -137,6 +137,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>user_id</t>
   </si>
 </sst>
 </file>
@@ -513,209 +516,227 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CC210C0-9D73-46BA-9C56-AD0FD5D86CE8}">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>5</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>33</v>
       </c>
-      <c r="J1" t="s">
-        <v>1</v>
-      </c>
       <c r="K1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
         <v>34</v>
       </c>
-      <c r="L2" s="1"/>
       <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="2">
+        <v>1</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="4"/>
       <c r="K3" s="4"/>
+      <c r="L3" s="4"/>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H4" s="2">
-        <v>1</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="2">
+        <v>1</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="4"/>
       <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>26</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="4">
-        <v>1</v>
-      </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="4">
+        <v>1</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="4"/>
       <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>30</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>31</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="H6" s="4">
-        <v>1</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="I6" s="4">
+        <v>1</v>
+      </c>
+      <c r="J6" s="4" t="s">
         <v>34</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G6" r:id="rId1" xr:uid="{B599CD98-9163-4B46-B2A9-E2071997EE60}"/>
-    <hyperlink ref="G5" r:id="rId2" xr:uid="{C74ED9C4-8AFE-4DA1-A2D6-E15B38EDC0CA}"/>
-    <hyperlink ref="G2" r:id="rId3" xr:uid="{F6913667-5CC3-40EA-B642-923A367E42BB}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{446F9170-EA64-4E96-B867-D0E06B099E8C}"/>
-    <hyperlink ref="G3" r:id="rId5" xr:uid="{B88822F8-8215-4151-AFB5-49CC67F7D085}"/>
+    <hyperlink ref="H6" r:id="rId1" xr:uid="{B599CD98-9163-4B46-B2A9-E2071997EE60}"/>
+    <hyperlink ref="H5" r:id="rId2" xr:uid="{C74ED9C4-8AFE-4DA1-A2D6-E15B38EDC0CA}"/>
+    <hyperlink ref="H2" r:id="rId3" xr:uid="{F6913667-5CC3-40EA-B642-923A367E42BB}"/>
+    <hyperlink ref="H4" r:id="rId4" xr:uid="{446F9170-EA64-4E96-B867-D0E06B099E8C}"/>
+    <hyperlink ref="H3" r:id="rId5" xr:uid="{B88822F8-8215-4151-AFB5-49CC67F7D085}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>